<commit_message>
Adding all the csvs
</commit_message>
<xml_diff>
--- a/BarbadosPlayers.xlsx
+++ b/BarbadosPlayers.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinheaney/Desktop/GitHub_Projects_Folder/Barbados_Turf_Club_Horse_Racing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{765D7995-E8EF-824E-A07A-79918DF2D1B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF849D2-B1F6-694A-9114-91E4D8A652C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="500" windowWidth="26140" windowHeight="14240" xr2:uid="{E5E74DBF-4C2C-0A42-87D7-4BBE1582C403}"/>
+    <workbookView xWindow="5300" yWindow="2460" windowWidth="26140" windowHeight="14240" activeTab="7" xr2:uid="{E5E74DBF-4C2C-0A42-87D7-4BBE1582C403}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Race1" sheetId="2" r:id="rId2"/>
+    <sheet name="Race2" sheetId="3" r:id="rId3"/>
+    <sheet name="Race3" sheetId="10" r:id="rId4"/>
+    <sheet name="Race4" sheetId="9" r:id="rId5"/>
+    <sheet name="Race5" sheetId="8" r:id="rId6"/>
+    <sheet name="Race6" sheetId="7" r:id="rId7"/>
+    <sheet name="Race7" sheetId="6" r:id="rId8"/>
+    <sheet name="Race 8" sheetId="5" r:id="rId9"/>
+    <sheet name="Race9" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="171">
   <si>
     <t>Natalie</t>
   </si>
@@ -237,6 +245,360 @@
   </si>
   <si>
     <t>(510) 409-9587</t>
+  </si>
+  <si>
+    <t>DE CONKIE MAN</t>
+  </si>
+  <si>
+    <t>ROCKIN ROBIN</t>
+  </si>
+  <si>
+    <t>MAKEDA(Res 01)</t>
+  </si>
+  <si>
+    <t>PETTICOAT</t>
+  </si>
+  <si>
+    <t>SARAH(T&amp;T)</t>
+  </si>
+  <si>
+    <t>THUNDER LADY</t>
+  </si>
+  <si>
+    <t>RACHEL(Res 02)</t>
+  </si>
+  <si>
+    <t>ONEBILLIONUS</t>
+  </si>
+  <si>
+    <t>JONAH</t>
+  </si>
+  <si>
+    <t>ANASTASIA</t>
+  </si>
+  <si>
+    <t>PEOPLE‚ÄôS CHAMP</t>
+  </si>
+  <si>
+    <t>CABALLITO(Res 05)</t>
+  </si>
+  <si>
+    <t>MIRIAM(Res 03)</t>
+  </si>
+  <si>
+    <t>UNGRATEFUL</t>
+  </si>
+  <si>
+    <t>DREAM SOCIETY</t>
+  </si>
+  <si>
+    <t>DE SPOILED CHILD(Res 04)</t>
+  </si>
+  <si>
+    <t>NO BOSS NO</t>
+  </si>
+  <si>
+    <t>AMEASH(Res 06)</t>
+  </si>
+  <si>
+    <t>PRETTY PRINCESS(Res 07)</t>
+  </si>
+  <si>
+    <t>GOLD STAR</t>
+  </si>
+  <si>
+    <t>ST. DAVIDS</t>
+  </si>
+  <si>
+    <t>OPRAH</t>
+  </si>
+  <si>
+    <t>SATIVA</t>
+  </si>
+  <si>
+    <t>TIGERS NEST</t>
+  </si>
+  <si>
+    <t>FILMORES(Res 04)</t>
+  </si>
+  <si>
+    <t>AERODYNAMIC</t>
+  </si>
+  <si>
+    <t>OBEROI(Res 02)</t>
+  </si>
+  <si>
+    <t>SILVER BULLET</t>
+  </si>
+  <si>
+    <t>RIDDICK</t>
+  </si>
+  <si>
+    <t>SAN PEDRO(Res 05)</t>
+  </si>
+  <si>
+    <t>BONITA BAY</t>
+  </si>
+  <si>
+    <t>HOWULIKEDISNAME</t>
+  </si>
+  <si>
+    <t>PROVENCE(Res 03)</t>
+  </si>
+  <si>
+    <t>ZENSATIONAL(Res 01)</t>
+  </si>
+  <si>
+    <t>SECRET MISSION</t>
+  </si>
+  <si>
+    <t>SCARFACE(Res 08)</t>
+  </si>
+  <si>
+    <t>AAZAM</t>
+  </si>
+  <si>
+    <t>LEADING STAR</t>
+  </si>
+  <si>
+    <t>PERUVIAN</t>
+  </si>
+  <si>
+    <t>GOLDEN TOUCH</t>
+  </si>
+  <si>
+    <t>PREMONITION</t>
+  </si>
+  <si>
+    <t>MISCHIEF MAKER</t>
+  </si>
+  <si>
+    <t>SEBASTIAN</t>
+  </si>
+  <si>
+    <t>FANTASTIC FRANCES</t>
+  </si>
+  <si>
+    <t>TROJAN</t>
+  </si>
+  <si>
+    <t>EDELWEISS(T&amp;T)</t>
+  </si>
+  <si>
+    <t>QUALITY STAR</t>
+  </si>
+  <si>
+    <t>WHATYOUTHINK</t>
+  </si>
+  <si>
+    <t>PRAY FOR ME</t>
+  </si>
+  <si>
+    <t>VISIONARY</t>
+  </si>
+  <si>
+    <t>NO FLY ZONE</t>
+  </si>
+  <si>
+    <t>KINGOFTHEVALLEY</t>
+  </si>
+  <si>
+    <t>GUEST AGAIN</t>
+  </si>
+  <si>
+    <t>BLACK ROCK</t>
+  </si>
+  <si>
+    <t>DONT DOUBT DORIS</t>
+  </si>
+  <si>
+    <t>LITTLE BUT LUCKY</t>
+  </si>
+  <si>
+    <t>FIRE CRACKER</t>
+  </si>
+  <si>
+    <t>BIRD CAGE</t>
+  </si>
+  <si>
+    <t>ODYSSEY</t>
+  </si>
+  <si>
+    <t>WATCHMESLEWDEM</t>
+  </si>
+  <si>
+    <t>JOUVERT</t>
+  </si>
+  <si>
+    <t>GABRIEL</t>
+  </si>
+  <si>
+    <t>PETER QUILL</t>
+  </si>
+  <si>
+    <t>BRIGHTON STAR</t>
+  </si>
+  <si>
+    <t>ALKORO(Res 03)</t>
+  </si>
+  <si>
+    <t>DARK ANGEL</t>
+  </si>
+  <si>
+    <t>TWINKLED</t>
+  </si>
+  <si>
+    <t>AGAINST HIS WILL</t>
+  </si>
+  <si>
+    <t>TAKE IT EASY</t>
+  </si>
+  <si>
+    <t>WHISPERING ANGEL(Res 01)</t>
+  </si>
+  <si>
+    <t>STEVENSONS THUNDER</t>
+  </si>
+  <si>
+    <t>SPARKLE(Res 02)</t>
+  </si>
+  <si>
+    <t>LADY BIRD</t>
+  </si>
+  <si>
+    <t>KARIBA STAR(USA)</t>
+  </si>
+  <si>
+    <t>STEALIN</t>
+  </si>
+  <si>
+    <t>MASARU(GB)</t>
+  </si>
+  <si>
+    <t>TRINI AVIATOR(USA)</t>
+  </si>
+  <si>
+    <t>ZAGAN(USA)</t>
+  </si>
+  <si>
+    <t>JOSHUA</t>
+  </si>
+  <si>
+    <t>SIR JIMMY(USA)</t>
+  </si>
+  <si>
+    <t>RADIAL FLYER(USA)</t>
+  </si>
+  <si>
+    <t>GANDALF</t>
+  </si>
+  <si>
+    <t>ISLAND COTTON(USA)</t>
+  </si>
+  <si>
+    <t>STOLEN</t>
+  </si>
+  <si>
+    <t>DEBONAIRE DAVID(GB)</t>
+  </si>
+  <si>
+    <t>AMANTE</t>
+  </si>
+  <si>
+    <t>ABSOLUT STAR</t>
+  </si>
+  <si>
+    <t>CRITERION</t>
+  </si>
+  <si>
+    <t>RACHEL</t>
+  </si>
+  <si>
+    <t>DEALWIDIT</t>
+  </si>
+  <si>
+    <t>MAKEDA</t>
+  </si>
+  <si>
+    <t>GAYZEE</t>
+  </si>
+  <si>
+    <t>QUEEN JUSTINA</t>
+  </si>
+  <si>
+    <t>TIME AFTER TIME</t>
+  </si>
+  <si>
+    <t>DOMINUS</t>
+  </si>
+  <si>
+    <t>FASTCASH</t>
+  </si>
+  <si>
+    <t>PREACHER BOY</t>
+  </si>
+  <si>
+    <t>STORM FORCE</t>
+  </si>
+  <si>
+    <t>TOOTIGHTTOTALK</t>
+  </si>
+  <si>
+    <t>CONFLICTOFINTEREST</t>
+  </si>
+  <si>
+    <t>LOLLIPOP(JAM)</t>
+  </si>
+  <si>
+    <t>ABIGAIL</t>
+  </si>
+  <si>
+    <t>MR. U S</t>
+  </si>
+  <si>
+    <t>ULTIMATE</t>
+  </si>
+  <si>
+    <t>RUTH</t>
+  </si>
+  <si>
+    <t>RIGHTONTIME(Res 01)</t>
+  </si>
+  <si>
+    <t>GAVILAR(USA)</t>
+  </si>
+  <si>
+    <t>TERRAIN(USA)</t>
+  </si>
+  <si>
+    <t>SHOTTA(USA)</t>
+  </si>
+  <si>
+    <t>JUNIPERO AVENUE(USA)</t>
+  </si>
+  <si>
+    <t>INSPIRED ADVENTURE(USA)</t>
+  </si>
+  <si>
+    <t>SEVENTEENMILLIONUS</t>
+  </si>
+  <si>
+    <t>GOOD VIBRATION</t>
+  </si>
+  <si>
+    <t>JACKMANANNYGAP</t>
+  </si>
+  <si>
+    <t>NEILOS</t>
+  </si>
+  <si>
+    <t>NASTY CRITTER</t>
+  </si>
+  <si>
+    <t>ORIENTAL CROWN</t>
+  </si>
+  <si>
+    <t>SING SING</t>
   </si>
 </sst>
 </file>
@@ -623,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3421611A-56EB-534E-BD24-0A5EA991AF56}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A29"/>
     </sheetView>
   </sheetViews>
@@ -702,19 +1064,19 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(1,17)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <f ca="1">RANDBETWEEN(1,13)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <f ca="1">RANDBETWEEN(1,8)</f>
@@ -722,19 +1084,19 @@
       </c>
       <c r="M2">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O2">
         <f ca="1">RANDBETWEEN(1,15)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q2">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S2">
         <f ca="1">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -746,39 +1108,39 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C29" ca="1" si="0">RANDBETWEEN(1,17)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E29" ca="1" si="1">RANDBETWEEN(1,20)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G29" ca="1" si="2">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I29" ca="1" si="3">RANDBETWEEN(1,13)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K28" ca="1" si="4">RANDBETWEEN(1,8)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M28" ca="1" si="5">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O28" ca="1" si="6">RANDBETWEEN(1,15)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q28" ca="1" si="7">RANDBETWEEN(1,9)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S28" ca="1" si="8">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -790,19 +1152,19 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
@@ -810,19 +1172,19 @@
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <f t="shared" ca="1" si="8"/>
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -834,19 +1196,19 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="4"/>
@@ -854,19 +1216,19 @@
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S5">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -878,27 +1240,27 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="6"/>
@@ -906,11 +1268,11 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="S6">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -922,19 +1284,19 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="4"/>
@@ -942,19 +1304,19 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="S7">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -966,15 +1328,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
@@ -982,19 +1344,19 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S8">
         <f t="shared" ca="1" si="8"/>
@@ -1010,39 +1372,39 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S9">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1054,35 +1416,35 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S10">
         <f t="shared" ca="1" si="8"/>
@@ -1098,23 +1460,23 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="5"/>
@@ -1122,15 +1484,15 @@
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S11">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1142,15 +1504,15 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="3"/>
@@ -1158,23 +1520,23 @@
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1186,35 +1548,35 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="8"/>
@@ -1230,39 +1592,39 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1274,7 +1636,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
@@ -1282,31 +1644,31 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O15">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="7"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1318,7 +1680,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
@@ -1326,27 +1688,27 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O16">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="8"/>
@@ -1362,19 +1724,19 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="4"/>
@@ -1382,11 +1744,11 @@
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O17">
         <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="7"/>
@@ -1394,7 +1756,7 @@
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
@@ -1406,39 +1768,39 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O18">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -1450,11 +1812,11 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
@@ -1462,15 +1824,15 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O19">
         <f t="shared" ca="1" si="6"/>
@@ -1478,11 +1840,11 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="7"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -1494,39 +1856,39 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M20">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O20">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S20">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
@@ -1538,23 +1900,23 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M21">
         <f t="shared" ca="1" si="5"/>
@@ -1562,15 +1924,15 @@
       </c>
       <c r="O21">
         <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S21">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
@@ -1582,11 +1944,11 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
@@ -1594,27 +1956,27 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M22">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O22">
         <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S22">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -1626,19 +1988,19 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="4"/>
@@ -1646,15 +2008,15 @@
       </c>
       <c r="M23">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="7"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="8"/>
@@ -1670,39 +2032,39 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M24">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O24">
         <f t="shared" ca="1" si="6"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="7"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S24">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -1714,39 +2076,39 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O25">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S25">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
@@ -1758,39 +2120,39 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M26">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O26">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="S26">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
@@ -1802,39 +2164,39 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M27">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="O27">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="7"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S27">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -1846,11 +2208,11 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="2"/>
@@ -1858,15 +2220,15 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O28">
         <f t="shared" ca="1" si="6"/>
@@ -1874,11 +2236,11 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="S28">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
@@ -1890,19 +2252,19 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1913,14 +2275,1081 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CD98E9-3C44-C44A-8DC0-3A60F2BAA1D8}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331E5179-35BE-4142-BCD9-CD69176886F8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D37052C-F253-EA41-92B9-740434BC63AA}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4B51C4-A818-C64A-80E3-91C1C38ACDC9}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247E0B5-44BE-F549-87F1-1DC7A7AE2F2D}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CECB5BA-C47D-034A-96A6-269D1D458915}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38354052-D548-9544-932E-AF6E28703C32}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9187E1-6B26-2F4D-A317-81E182A869D0}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E326321B-9993-6B4B-AAE7-67DD37CCE8B8}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>